<commit_message>
add missing partof data
</commit_message>
<xml_diff>
--- a/dataSet.xlsx
+++ b/dataSet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/legend/QoL-main/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEFD5EC4-CF15-DF45-8459-EC0988444551}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BC60C61-932A-854F-B6AF-CBF017C55157}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18520" yWindow="2640" windowWidth="40600" windowHeight="23980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="680" yWindow="1980" windowWidth="40600" windowHeight="23980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1250,8 +1250,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z479"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="A52" sqref="A52:XFD52"/>
+    <sheetView tabSelected="1" topLeftCell="A333" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="E67" sqref="E67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4626,6 +4626,9 @@
       <c r="D52" s="3" t="s">
         <v>139</v>
       </c>
+      <c r="E52">
+        <v>4</v>
+      </c>
       <c r="F52">
         <v>2</v>
       </c>
@@ -4819,6 +4822,9 @@
       <c r="D55" s="3" t="s">
         <v>140</v>
       </c>
+      <c r="E55">
+        <v>4</v>
+      </c>
       <c r="F55">
         <v>2</v>
       </c>
@@ -5013,6 +5019,9 @@
       <c r="D58" s="3" t="s">
         <v>15</v>
       </c>
+      <c r="E58">
+        <v>4</v>
+      </c>
       <c r="F58">
         <v>2</v>
       </c>
@@ -5206,6 +5215,9 @@
       <c r="D61" s="3" t="s">
         <v>16</v>
       </c>
+      <c r="E61">
+        <v>4</v>
+      </c>
       <c r="F61">
         <v>2</v>
       </c>
@@ -5399,6 +5411,9 @@
       <c r="D64" s="3" t="s">
         <v>17</v>
       </c>
+      <c r="E64">
+        <v>4</v>
+      </c>
       <c r="F64">
         <v>2</v>
       </c>
@@ -5591,6 +5606,9 @@
       </c>
       <c r="D67" s="3" t="s">
         <v>141</v>
+      </c>
+      <c r="E67">
+        <v>4</v>
       </c>
       <c r="F67">
         <v>2</v>

</xml_diff>